<commit_message>
feat: create endpoint for uploading FFMM Excel (update existing entries and create new ones)
</commit_message>
<xml_diff>
--- a/src/assets/Excel-FFMM.xlsx
+++ b/src/assets/Excel-FFMM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\practicantecomercial\FFMM-backend\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C5E107-6C47-45B1-9EAB-7A5CA19F3D2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69ACED6A-A417-4418-89D0-CD51F6BF0965}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{8B08BC30-49CD-40DC-BE07-9829148F593A}"/>
   </bookViews>
@@ -932,7 +932,7 @@
     <t>Alto</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>Link ficha</t>
   </si>
 </sst>
 </file>
@@ -1437,17 +1437,17 @@
   <dimension ref="A1:N278"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C159" sqref="C159"/>
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -1488,10 +1488,10 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>4</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>6</v>
@@ -1523,10 +1523,10 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>9</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>10</v>
@@ -1557,10 +1557,10 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4"/>
+      <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="2" t="s">
         <v>7</v>
@@ -1589,10 +1589,10 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>12</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>13</v>
@@ -1623,10 +1623,10 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4"/>
+      <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="2" t="s">
         <v>11</v>
@@ -1655,10 +1655,10 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>16</v>
@@ -1689,10 +1689,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="4"/>
+      <c r="B8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="2" t="s">
         <v>11</v>
@@ -1720,10 +1720,10 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="4"/>
+      <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="2" t="s">
         <v>17</v>
@@ -1751,10 +1751,10 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="4"/>
+      <c r="B10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="2" t="s">
         <v>18</v>
@@ -1783,10 +1783,10 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>19</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>20</v>
@@ -1817,10 +1817,10 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="4"/>
+      <c r="B12" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="2" t="s">
         <v>11</v>
@@ -1849,10 +1849,10 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>22</v>
@@ -1884,10 +1884,10 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>24</v>
@@ -1919,10 +1919,10 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>26</v>
@@ -1954,10 +1954,10 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>28</v>
@@ -1988,10 +1988,10 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="4"/>
+      <c r="B17" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="2" t="s">
         <v>11</v>
@@ -2020,10 +2020,10 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>30</v>
@@ -2054,10 +2054,10 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="4"/>
+      <c r="B19" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="2" t="s">
         <v>11</v>
@@ -2086,10 +2086,10 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>32</v>
@@ -2120,10 +2120,10 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="4"/>
+      <c r="B21" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="2" t="s">
         <v>11</v>
@@ -2152,10 +2152,10 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>34</v>
@@ -2186,10 +2186,10 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="4"/>
+      <c r="B23" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="2" t="s">
         <v>11</v>
@@ -2218,10 +2218,10 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>36</v>
@@ -2252,10 +2252,10 @@
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="4"/>
+      <c r="B25" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="2" t="s">
         <v>11</v>
@@ -2284,10 +2284,10 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>37</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>38</v>
@@ -2318,10 +2318,10 @@
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3" t="s">
         <v>11</v>
@@ -2350,10 +2350,10 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>40</v>
@@ -2384,10 +2384,10 @@
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3" t="s">
         <v>11</v>
@@ -2416,10 +2416,10 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>42</v>
@@ -2451,10 +2451,10 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>44</v>
@@ -2486,10 +2486,10 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>45</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>46</v>
@@ -2521,10 +2521,10 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>47</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>48</v>
@@ -2556,10 +2556,10 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>49</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>50</v>
@@ -2591,10 +2591,10 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>52</v>
@@ -2626,10 +2626,10 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>53</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>54</v>
@@ -2660,10 +2660,10 @@
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
+      <c r="A37" s="4"/>
+      <c r="B37" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B37" s="4"/>
       <c r="C37" s="4"/>
       <c r="D37" s="2" t="s">
         <v>11</v>
@@ -2692,10 +2692,10 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>55</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>56</v>
@@ -2726,10 +2726,10 @@
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="4"/>
+      <c r="B39" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B39" s="4"/>
       <c r="C39" s="4"/>
       <c r="D39" s="2" t="s">
         <v>11</v>
@@ -2758,10 +2758,10 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B40" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>57</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>58</v>
@@ -2793,10 +2793,10 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B41" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>59</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>60</v>
@@ -2828,10 +2828,10 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B42" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>61</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>62</v>
@@ -2863,10 +2863,10 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B43" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>63</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>64</v>
@@ -2898,10 +2898,10 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B44" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>65</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>66</v>
@@ -2933,10 +2933,10 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B45" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>68</v>
@@ -2968,10 +2968,10 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B46" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>69</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>70</v>
@@ -3003,10 +3003,10 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B47" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>71</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>72</v>
@@ -3038,10 +3038,10 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B48" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>73</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>74</v>
@@ -3073,10 +3073,10 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B49" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>75</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>76</v>
@@ -3107,10 +3107,10 @@
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
+      <c r="A50" s="4"/>
+      <c r="B50" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B50" s="4"/>
       <c r="C50" s="4"/>
       <c r="D50" s="2" t="s">
         <v>11</v>
@@ -3139,10 +3139,10 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B51" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>77</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>78</v>
@@ -3173,10 +3173,10 @@
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
+      <c r="A52" s="4"/>
+      <c r="B52" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B52" s="4"/>
       <c r="C52" s="4"/>
       <c r="D52" s="2" t="s">
         <v>11</v>
@@ -3205,10 +3205,10 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B53" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>79</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>80</v>
@@ -3239,10 +3239,10 @@
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
+      <c r="A54" s="4"/>
+      <c r="B54" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B54" s="4"/>
       <c r="C54" s="4"/>
       <c r="D54" s="2" t="s">
         <v>11</v>
@@ -3271,10 +3271,10 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B55" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>82</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>83</v>
@@ -3302,10 +3302,10 @@
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
+      <c r="A56" s="4"/>
+      <c r="B56" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B56" s="4"/>
       <c r="C56" s="4"/>
       <c r="D56" s="2" t="s">
         <v>11</v>
@@ -3333,10 +3333,10 @@
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="3" t="s">
+      <c r="A57" s="4"/>
+      <c r="B57" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B57" s="4"/>
       <c r="C57" s="4"/>
       <c r="D57" s="2" t="s">
         <v>84</v>
@@ -3365,10 +3365,10 @@
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B58" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>85</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>86</v>
@@ -3399,10 +3399,10 @@
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A59" s="3" t="s">
+      <c r="A59" s="4"/>
+      <c r="B59" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B59" s="4"/>
       <c r="C59" s="4"/>
       <c r="D59" s="2" t="s">
         <v>11</v>
@@ -3431,10 +3431,10 @@
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B60" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>87</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>88</v>
@@ -3466,10 +3466,10 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B61" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>89</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>90</v>
@@ -3501,10 +3501,10 @@
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B62" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>92</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>93</v>
@@ -3535,10 +3535,10 @@
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A63" s="3" t="s">
+      <c r="A63" s="4"/>
+      <c r="B63" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B63" s="4"/>
       <c r="C63" s="4"/>
       <c r="D63" s="2" t="s">
         <v>11</v>
@@ -3567,10 +3567,10 @@
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B64" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>94</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>95</v>
@@ -3601,10 +3601,10 @@
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A65" s="3" t="s">
+      <c r="A65" s="4"/>
+      <c r="B65" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B65" s="4"/>
       <c r="C65" s="4"/>
       <c r="D65" s="2" t="s">
         <v>11</v>
@@ -3633,10 +3633,10 @@
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B66" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>96</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>97</v>
@@ -3667,10 +3667,10 @@
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A67" s="3" t="s">
+      <c r="A67" s="4"/>
+      <c r="B67" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B67" s="4"/>
       <c r="C67" s="4"/>
       <c r="D67" s="2" t="s">
         <v>11</v>
@@ -3699,10 +3699,10 @@
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B68" s="3" t="s">
         <v>98</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>99</v>
       </c>
       <c r="C68" s="3" t="s">
         <v>100</v>
@@ -3734,10 +3734,10 @@
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B69" s="3" t="s">
         <v>98</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>101</v>
       </c>
       <c r="C69" s="3" t="s">
         <v>102</v>
@@ -3769,10 +3769,10 @@
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B70" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>104</v>
       </c>
       <c r="C70" s="3" t="s">
         <v>105</v>
@@ -3803,10 +3803,10 @@
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A71" s="3" t="s">
+      <c r="A71" s="4"/>
+      <c r="B71" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B71" s="4"/>
       <c r="C71" s="4"/>
       <c r="D71" s="2" t="s">
         <v>106</v>
@@ -3834,10 +3834,10 @@
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A72" s="3" t="s">
+      <c r="A72" s="4"/>
+      <c r="B72" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B72" s="4"/>
       <c r="C72" s="4"/>
       <c r="D72" s="2" t="s">
         <v>107</v>
@@ -3865,10 +3865,10 @@
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A73" s="3" t="s">
+      <c r="A73" s="4"/>
+      <c r="B73" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B73" s="4"/>
       <c r="C73" s="4"/>
       <c r="D73" s="2" t="s">
         <v>108</v>
@@ -3897,10 +3897,10 @@
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B74" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>109</v>
       </c>
       <c r="C74" s="3" t="s">
         <v>110</v>
@@ -3931,10 +3931,10 @@
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A75" s="3" t="s">
+      <c r="A75" s="4"/>
+      <c r="B75" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B75" s="4"/>
       <c r="C75" s="4"/>
       <c r="D75" s="2" t="s">
         <v>106</v>
@@ -3962,10 +3962,10 @@
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A76" s="3" t="s">
+      <c r="A76" s="4"/>
+      <c r="B76" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B76" s="4"/>
       <c r="C76" s="4"/>
       <c r="D76" s="2" t="s">
         <v>107</v>
@@ -3993,10 +3993,10 @@
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A77" s="3" t="s">
+      <c r="A77" s="4"/>
+      <c r="B77" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B77" s="4"/>
       <c r="C77" s="4"/>
       <c r="D77" s="2" t="s">
         <v>108</v>
@@ -4025,10 +4025,10 @@
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B78" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>111</v>
       </c>
       <c r="C78" s="3" t="s">
         <v>112</v>
@@ -4059,10 +4059,10 @@
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A79" s="3" t="s">
+      <c r="A79" s="4"/>
+      <c r="B79" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B79" s="4"/>
       <c r="C79" s="4"/>
       <c r="D79" s="2" t="s">
         <v>106</v>
@@ -4090,10 +4090,10 @@
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A80" s="3" t="s">
+      <c r="A80" s="4"/>
+      <c r="B80" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B80" s="4"/>
       <c r="C80" s="4"/>
       <c r="D80" s="2" t="s">
         <v>107</v>
@@ -4120,8 +4120,8 @@
         <v>295</v>
       </c>
     </row>
-    <row r="81" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B81" s="4"/>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A81" s="4"/>
       <c r="C81" s="4"/>
       <c r="D81" s="2" t="s">
         <v>108</v>
@@ -4148,8 +4148,8 @@
         <v>295</v>
       </c>
     </row>
-    <row r="82" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B82" s="3" t="s">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A82" s="3" t="s">
         <v>113</v>
       </c>
       <c r="C82" s="3" t="s">
@@ -4180,8 +4180,8 @@
         <v>295</v>
       </c>
     </row>
-    <row r="83" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B83" s="4"/>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A83" s="4"/>
       <c r="C83" s="4"/>
       <c r="D83" s="2" t="s">
         <v>106</v>
@@ -4208,8 +4208,8 @@
         <v>295</v>
       </c>
     </row>
-    <row r="84" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B84" s="4"/>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A84" s="4"/>
       <c r="C84" s="4"/>
       <c r="D84" s="2" t="s">
         <v>107</v>
@@ -4236,8 +4236,8 @@
         <v>295</v>
       </c>
     </row>
-    <row r="85" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B85" s="4"/>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A85" s="4"/>
       <c r="C85" s="4"/>
       <c r="D85" s="2" t="s">
         <v>108</v>
@@ -4264,8 +4264,8 @@
         <v>295</v>
       </c>
     </row>
-    <row r="86" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B86" s="3" t="s">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A86" s="3" t="s">
         <v>115</v>
       </c>
       <c r="C86" s="3" t="s">
@@ -4296,8 +4296,8 @@
         <v>295</v>
       </c>
     </row>
-    <row r="87" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B87" s="4"/>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A87" s="4"/>
       <c r="C87" s="4"/>
       <c r="D87" s="2" t="s">
         <v>106</v>
@@ -4324,8 +4324,8 @@
         <v>295</v>
       </c>
     </row>
-    <row r="88" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B88" s="4"/>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A88" s="4"/>
       <c r="C88" s="4"/>
       <c r="D88" s="2" t="s">
         <v>117</v>
@@ -4352,8 +4352,8 @@
         <v>295</v>
       </c>
     </row>
-    <row r="89" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B89" s="4"/>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A89" s="4"/>
       <c r="C89" s="4"/>
       <c r="D89" s="2" t="s">
         <v>107</v>
@@ -4380,8 +4380,8 @@
         <v>295</v>
       </c>
     </row>
-    <row r="90" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B90" s="4"/>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A90" s="4"/>
       <c r="C90" s="4"/>
       <c r="D90" s="2" t="s">
         <v>108</v>
@@ -4408,8 +4408,8 @@
         <v>295</v>
       </c>
     </row>
-    <row r="91" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B91" s="3" t="s">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A91" s="3" t="s">
         <v>118</v>
       </c>
       <c r="C91" s="3" t="s">
@@ -4440,8 +4440,8 @@
         <v>295</v>
       </c>
     </row>
-    <row r="92" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B92" s="4"/>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A92" s="4"/>
       <c r="C92" s="4"/>
       <c r="D92" s="2" t="s">
         <v>106</v>
@@ -4468,8 +4468,8 @@
         <v>295</v>
       </c>
     </row>
-    <row r="93" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B93" s="4"/>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A93" s="4"/>
       <c r="C93" s="4"/>
       <c r="D93" s="2" t="s">
         <v>107</v>
@@ -4496,8 +4496,8 @@
         <v>295</v>
       </c>
     </row>
-    <row r="94" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B94" s="4"/>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A94" s="4"/>
       <c r="C94" s="4"/>
       <c r="D94" s="2" t="s">
         <v>108</v>
@@ -4524,8 +4524,8 @@
         <v>295</v>
       </c>
     </row>
-    <row r="95" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B95" s="3" t="s">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A95" s="3" t="s">
         <v>120</v>
       </c>
       <c r="C95" s="3" t="s">
@@ -4556,8 +4556,8 @@
         <v>295</v>
       </c>
     </row>
-    <row r="96" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B96" s="4"/>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A96" s="4"/>
       <c r="C96" s="4"/>
       <c r="D96" s="2" t="s">
         <v>107</v>
@@ -4585,7 +4585,7 @@
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B97" s="4"/>
+      <c r="A97" s="4"/>
       <c r="C97" s="4"/>
       <c r="D97" s="2" t="s">
         <v>108</v>
@@ -4613,7 +4613,7 @@
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B98" s="3" t="s">
+      <c r="A98" s="3" t="s">
         <v>122</v>
       </c>
       <c r="C98" s="3" t="s">
@@ -4645,7 +4645,7 @@
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B99" s="3" t="s">
+      <c r="A99" s="3" t="s">
         <v>124</v>
       </c>
       <c r="C99" s="3" t="s">
@@ -4677,7 +4677,7 @@
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B100" s="4"/>
+      <c r="A100" s="4"/>
       <c r="C100" s="4"/>
       <c r="D100" s="2" t="s">
         <v>106</v>
@@ -4705,7 +4705,7 @@
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B101" s="4"/>
+      <c r="A101" s="4"/>
       <c r="C101" s="4"/>
       <c r="D101" s="2" t="s">
         <v>107</v>
@@ -4733,7 +4733,7 @@
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B102" s="4"/>
+      <c r="A102" s="4"/>
       <c r="C102" s="4"/>
       <c r="D102" s="2" t="s">
         <v>108</v>
@@ -4761,7 +4761,7 @@
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B103" s="3" t="s">
+      <c r="A103" s="3" t="s">
         <v>126</v>
       </c>
       <c r="C103" s="3" t="s">
@@ -4793,7 +4793,7 @@
       </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B104" s="4"/>
+      <c r="A104" s="4"/>
       <c r="C104" s="4"/>
       <c r="D104" s="2" t="s">
         <v>106</v>
@@ -4821,7 +4821,7 @@
       </c>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B105" s="4"/>
+      <c r="A105" s="4"/>
       <c r="C105" s="4"/>
       <c r="D105" s="2" t="s">
         <v>107</v>
@@ -4849,7 +4849,7 @@
       </c>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B106" s="4"/>
+      <c r="A106" s="4"/>
       <c r="C106" s="4"/>
       <c r="D106" s="2" t="s">
         <v>108</v>
@@ -4877,7 +4877,7 @@
       </c>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B107" s="3" t="s">
+      <c r="A107" s="3" t="s">
         <v>128</v>
       </c>
       <c r="C107" s="3" t="s">
@@ -4909,7 +4909,7 @@
       </c>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B108" s="4"/>
+      <c r="A108" s="4"/>
       <c r="C108" s="4"/>
       <c r="D108" s="2" t="s">
         <v>106</v>
@@ -4937,7 +4937,7 @@
       </c>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B109" s="4"/>
+      <c r="A109" s="4"/>
       <c r="C109" s="4"/>
       <c r="D109" s="2" t="s">
         <v>107</v>
@@ -4965,7 +4965,7 @@
       </c>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B110" s="4"/>
+      <c r="A110" s="4"/>
       <c r="C110" s="4"/>
       <c r="D110" s="2" t="s">
         <v>108</v>
@@ -4993,10 +4993,10 @@
       </c>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A111" s="4"/>
-      <c r="B111" s="3" t="s">
+      <c r="A111" s="3" t="s">
         <v>130</v>
       </c>
+      <c r="B111" s="4"/>
       <c r="C111" s="3" t="s">
         <v>131</v>
       </c>
@@ -5113,10 +5113,10 @@
       </c>
     </row>
     <row r="115" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A115" s="4"/>
-      <c r="B115" s="3" t="s">
+      <c r="A115" s="3" t="s">
         <v>132</v>
       </c>
+      <c r="B115" s="4"/>
       <c r="C115" s="3" t="s">
         <v>133</v>
       </c>
@@ -5233,10 +5233,10 @@
       </c>
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A119" s="4"/>
-      <c r="B119" s="3" t="s">
+      <c r="A119" s="3" t="s">
         <v>134</v>
       </c>
+      <c r="B119" s="4"/>
       <c r="C119" s="3" t="s">
         <v>135</v>
       </c>
@@ -5353,10 +5353,10 @@
       </c>
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A123" s="4"/>
-      <c r="B123" s="3" t="s">
+      <c r="A123" s="3" t="s">
         <v>136</v>
       </c>
+      <c r="B123" s="4"/>
       <c r="C123" s="3" t="s">
         <v>137</v>
       </c>
@@ -5502,10 +5502,10 @@
       </c>
     </row>
     <row r="128" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A128" s="4"/>
-      <c r="B128" s="3" t="s">
+      <c r="A128" s="3" t="s">
         <v>138</v>
       </c>
+      <c r="B128" s="4"/>
       <c r="C128" s="3" t="s">
         <v>139</v>
       </c>
@@ -5651,10 +5651,10 @@
       </c>
     </row>
     <row r="133" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A133" s="4"/>
-      <c r="B133" s="3" t="s">
+      <c r="A133" s="3" t="s">
         <v>140</v>
       </c>
+      <c r="B133" s="4"/>
       <c r="C133" s="3" t="s">
         <v>141</v>
       </c>
@@ -5800,10 +5800,10 @@
       </c>
     </row>
     <row r="138" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A138" s="4"/>
-      <c r="B138" s="3" t="s">
+      <c r="A138" s="3" t="s">
         <v>142</v>
       </c>
+      <c r="B138" s="4"/>
       <c r="C138" s="3" t="s">
         <v>143</v>
       </c>
@@ -5920,10 +5920,10 @@
       </c>
     </row>
     <row r="142" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A142" s="4"/>
-      <c r="B142" s="3" t="s">
+      <c r="A142" s="3" t="s">
         <v>144</v>
       </c>
+      <c r="B142" s="4"/>
       <c r="C142" s="3" t="s">
         <v>145</v>
       </c>
@@ -6040,10 +6040,10 @@
       </c>
     </row>
     <row r="146" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A146" s="4"/>
-      <c r="B146" s="3" t="s">
+      <c r="A146" s="3" t="s">
         <v>146</v>
       </c>
+      <c r="B146" s="4"/>
       <c r="C146" s="3" t="s">
         <v>147</v>
       </c>
@@ -6189,10 +6189,10 @@
       </c>
     </row>
     <row r="151" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A151" s="4"/>
-      <c r="B151" s="3" t="s">
+      <c r="A151" s="3" t="s">
         <v>148</v>
       </c>
+      <c r="B151" s="4"/>
       <c r="C151" s="3" t="s">
         <v>149</v>
       </c>
@@ -6310,10 +6310,10 @@
     </row>
     <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B155" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="B155" s="3" t="s">
-        <v>150</v>
       </c>
       <c r="C155" s="3" t="s">
         <v>151</v>
@@ -6345,10 +6345,10 @@
     </row>
     <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B156" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="B156" s="3" t="s">
-        <v>150</v>
       </c>
       <c r="C156" s="4"/>
       <c r="D156" s="2" t="s">
@@ -6378,10 +6378,10 @@
     </row>
     <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B157" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="B157" s="3" t="s">
-        <v>150</v>
       </c>
       <c r="C157" s="4"/>
       <c r="D157" s="2" t="s">
@@ -6411,10 +6411,10 @@
     </row>
     <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B158" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="B158" s="3" t="s">
-        <v>150</v>
       </c>
       <c r="C158" s="4"/>
       <c r="D158" s="2" t="s">
@@ -6444,10 +6444,10 @@
     </row>
     <row r="159" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A159" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B159" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="B159" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="C159" s="3" t="s">
         <v>153</v>
@@ -6479,10 +6479,10 @@
     </row>
     <row r="160" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A160" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B160" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="B160" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="C160" s="4"/>
       <c r="D160" s="2" t="s">
@@ -6512,10 +6512,10 @@
     </row>
     <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B161" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="B161" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="C161" s="4"/>
       <c r="D161" s="2" t="s">
@@ -6545,10 +6545,10 @@
     </row>
     <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B162" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="B162" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="C162" s="4"/>
       <c r="D162" s="2" t="s">
@@ -6578,10 +6578,10 @@
     </row>
     <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B163" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="B163" s="3" t="s">
-        <v>154</v>
       </c>
       <c r="C163" s="3" t="s">
         <v>155</v>
@@ -6612,10 +6612,10 @@
       </c>
     </row>
     <row r="164" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A164" s="3" t="s">
+      <c r="A164" s="4"/>
+      <c r="B164" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B164" s="4"/>
       <c r="C164" s="4"/>
       <c r="D164" s="2" t="s">
         <v>106</v>
@@ -6643,10 +6643,10 @@
       </c>
     </row>
     <row r="165" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A165" s="3" t="s">
+      <c r="A165" s="4"/>
+      <c r="B165" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B165" s="4"/>
       <c r="C165" s="4"/>
       <c r="D165" s="2" t="s">
         <v>117</v>
@@ -6674,10 +6674,10 @@
       </c>
     </row>
     <row r="166" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A166" s="3" t="s">
+      <c r="A166" s="4"/>
+      <c r="B166" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B166" s="4"/>
       <c r="C166" s="4"/>
       <c r="D166" s="2" t="s">
         <v>107</v>
@@ -6705,10 +6705,10 @@
       </c>
     </row>
     <row r="167" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A167" s="3" t="s">
+      <c r="A167" s="4"/>
+      <c r="B167" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B167" s="4"/>
       <c r="C167" s="4"/>
       <c r="D167" s="2" t="s">
         <v>108</v>
@@ -6737,10 +6737,10 @@
     </row>
     <row r="168" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A168" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B168" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="B168" s="3" t="s">
-        <v>156</v>
       </c>
       <c r="C168" s="3" t="s">
         <v>157</v>
@@ -6771,10 +6771,10 @@
       </c>
     </row>
     <row r="169" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A169" s="3" t="s">
+      <c r="A169" s="4"/>
+      <c r="B169" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B169" s="4"/>
       <c r="C169" s="4"/>
       <c r="D169" s="2" t="s">
         <v>106</v>
@@ -6802,10 +6802,10 @@
       </c>
     </row>
     <row r="170" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A170" s="3" t="s">
+      <c r="A170" s="4"/>
+      <c r="B170" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B170" s="4"/>
       <c r="C170" s="4"/>
       <c r="D170" s="2" t="s">
         <v>107</v>
@@ -6833,10 +6833,10 @@
       </c>
     </row>
     <row r="171" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A171" s="3" t="s">
+      <c r="A171" s="4"/>
+      <c r="B171" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B171" s="4"/>
       <c r="C171" s="4"/>
       <c r="D171" s="2" t="s">
         <v>108</v>
@@ -6865,10 +6865,10 @@
     </row>
     <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A172" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B172" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="B172" s="3" t="s">
-        <v>158</v>
       </c>
       <c r="C172" s="3" t="s">
         <v>159</v>
@@ -6899,10 +6899,10 @@
       </c>
     </row>
     <row r="173" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A173" s="3" t="s">
+      <c r="A173" s="4"/>
+      <c r="B173" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B173" s="4"/>
       <c r="C173" s="4"/>
       <c r="D173" s="2" t="s">
         <v>106</v>
@@ -6930,10 +6930,10 @@
       </c>
     </row>
     <row r="174" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A174" s="3" t="s">
+      <c r="A174" s="4"/>
+      <c r="B174" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B174" s="4"/>
       <c r="C174" s="4"/>
       <c r="D174" s="2" t="s">
         <v>107</v>
@@ -6961,10 +6961,10 @@
       </c>
     </row>
     <row r="175" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A175" s="3" t="s">
+      <c r="A175" s="4"/>
+      <c r="B175" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B175" s="4"/>
       <c r="C175" s="4"/>
       <c r="D175" s="2" t="s">
         <v>108</v>
@@ -6993,10 +6993,10 @@
     </row>
     <row r="176" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A176" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B176" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="B176" s="3" t="s">
-        <v>160</v>
       </c>
       <c r="C176" s="3" t="s">
         <v>161</v>
@@ -7027,10 +7027,10 @@
       </c>
     </row>
     <row r="177" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A177" s="3" t="s">
+      <c r="A177" s="4"/>
+      <c r="B177" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B177" s="4"/>
       <c r="C177" s="4"/>
       <c r="D177" s="2" t="s">
         <v>106</v>
@@ -7058,10 +7058,10 @@
       </c>
     </row>
     <row r="178" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A178" s="3" t="s">
+      <c r="A178" s="4"/>
+      <c r="B178" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B178" s="4"/>
       <c r="C178" s="4"/>
       <c r="D178" s="2" t="s">
         <v>107</v>
@@ -7089,10 +7089,10 @@
       </c>
     </row>
     <row r="179" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A179" s="3" t="s">
+      <c r="A179" s="4"/>
+      <c r="B179" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B179" s="4"/>
       <c r="C179" s="4"/>
       <c r="D179" s="2" t="s">
         <v>108</v>
@@ -7121,10 +7121,10 @@
     </row>
     <row r="180" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A180" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B180" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="B180" s="3" t="s">
-        <v>162</v>
       </c>
       <c r="C180" s="3" t="s">
         <v>163</v>
@@ -7155,10 +7155,10 @@
       </c>
     </row>
     <row r="181" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A181" s="3" t="s">
+      <c r="A181" s="4"/>
+      <c r="B181" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B181" s="4"/>
       <c r="C181" s="4"/>
       <c r="D181" s="2" t="s">
         <v>106</v>
@@ -7186,10 +7186,10 @@
       </c>
     </row>
     <row r="182" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A182" s="3" t="s">
+      <c r="A182" s="4"/>
+      <c r="B182" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B182" s="4"/>
       <c r="C182" s="4"/>
       <c r="D182" s="2" t="s">
         <v>117</v>
@@ -7217,10 +7217,10 @@
       </c>
     </row>
     <row r="183" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A183" s="3" t="s">
+      <c r="A183" s="4"/>
+      <c r="B183" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B183" s="4"/>
       <c r="C183" s="4"/>
       <c r="D183" s="2" t="s">
         <v>107</v>
@@ -7248,10 +7248,10 @@
       </c>
     </row>
     <row r="184" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A184" s="3" t="s">
+      <c r="A184" s="4"/>
+      <c r="B184" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B184" s="4"/>
       <c r="C184" s="4"/>
       <c r="D184" s="2" t="s">
         <v>108</v>
@@ -7280,10 +7280,10 @@
     </row>
     <row r="185" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A185" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B185" s="3" t="s">
         <v>164</v>
-      </c>
-      <c r="B185" s="3" t="s">
-        <v>165</v>
       </c>
       <c r="C185" s="3" t="s">
         <v>166</v>
@@ -7315,10 +7315,10 @@
     </row>
     <row r="186" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A186" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B186" s="3" t="s">
         <v>164</v>
-      </c>
-      <c r="B186" s="3" t="s">
-        <v>167</v>
       </c>
       <c r="C186" s="3" t="s">
         <v>168</v>
@@ -7350,10 +7350,10 @@
     </row>
     <row r="187" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A187" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B187" s="3" t="s">
         <v>164</v>
-      </c>
-      <c r="B187" s="3" t="s">
-        <v>169</v>
       </c>
       <c r="C187" s="3" t="s">
         <v>170</v>
@@ -7385,10 +7385,10 @@
     </row>
     <row r="188" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A188" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B188" s="3" t="s">
         <v>164</v>
-      </c>
-      <c r="B188" s="3" t="s">
-        <v>171</v>
       </c>
       <c r="C188" s="3" t="s">
         <v>172</v>
@@ -7420,10 +7420,10 @@
     </row>
     <row r="189" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A189" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B189" s="3" t="s">
         <v>164</v>
-      </c>
-      <c r="B189" s="3" t="s">
-        <v>173</v>
       </c>
       <c r="C189" s="3" t="s">
         <v>174</v>
@@ -7455,10 +7455,10 @@
     </row>
     <row r="190" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A190" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B190" s="3" t="s">
         <v>164</v>
-      </c>
-      <c r="B190" s="3" t="s">
-        <v>175</v>
       </c>
       <c r="C190" s="3" t="s">
         <v>176</v>
@@ -7490,10 +7490,10 @@
     </row>
     <row r="191" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A191" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B191" s="3" t="s">
         <v>177</v>
-      </c>
-      <c r="B191" s="3" t="s">
-        <v>178</v>
       </c>
       <c r="C191" s="3" t="s">
         <v>179</v>
@@ -7524,10 +7524,10 @@
       </c>
     </row>
     <row r="192" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A192" s="3" t="s">
+      <c r="A192" s="4"/>
+      <c r="B192" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B192" s="4"/>
       <c r="C192" s="4"/>
       <c r="D192" s="2" t="s">
         <v>180</v>
@@ -7555,10 +7555,10 @@
       </c>
     </row>
     <row r="193" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A193" s="3" t="s">
+      <c r="A193" s="4"/>
+      <c r="B193" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B193" s="4"/>
       <c r="C193" s="4"/>
       <c r="D193" s="2" t="s">
         <v>181</v>
@@ -7587,10 +7587,10 @@
     </row>
     <row r="194" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A194" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B194" s="3" t="s">
         <v>177</v>
-      </c>
-      <c r="B194" s="3" t="s">
-        <v>182</v>
       </c>
       <c r="C194" s="3" t="s">
         <v>183</v>
@@ -7621,10 +7621,10 @@
       </c>
     </row>
     <row r="195" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A195" s="3" t="s">
+      <c r="A195" s="4"/>
+      <c r="B195" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B195" s="4"/>
       <c r="C195" s="4"/>
       <c r="D195" s="2" t="s">
         <v>180</v>
@@ -7652,10 +7652,10 @@
       </c>
     </row>
     <row r="196" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A196" s="3" t="s">
+      <c r="A196" s="4"/>
+      <c r="B196" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B196" s="4"/>
       <c r="C196" s="4"/>
       <c r="D196" s="2" t="s">
         <v>181</v>
@@ -7684,10 +7684,10 @@
     </row>
     <row r="197" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A197" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B197" s="3" t="s">
         <v>177</v>
-      </c>
-      <c r="B197" s="3" t="s">
-        <v>184</v>
       </c>
       <c r="C197" s="3" t="s">
         <v>185</v>
@@ -7718,10 +7718,10 @@
       </c>
     </row>
     <row r="198" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A198" s="3" t="s">
+      <c r="A198" s="4"/>
+      <c r="B198" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B198" s="4"/>
       <c r="C198" s="4"/>
       <c r="D198" s="2" t="s">
         <v>186</v>
@@ -7749,10 +7749,10 @@
       </c>
     </row>
     <row r="199" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A199" s="3" t="s">
+      <c r="A199" s="4"/>
+      <c r="B199" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B199" s="4"/>
       <c r="C199" s="4"/>
       <c r="D199" s="2" t="s">
         <v>180</v>
@@ -7780,10 +7780,10 @@
       </c>
     </row>
     <row r="200" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A200" s="3" t="s">
+      <c r="A200" s="4"/>
+      <c r="B200" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B200" s="4"/>
       <c r="C200" s="4"/>
       <c r="D200" s="2" t="s">
         <v>181</v>
@@ -7812,10 +7812,10 @@
     </row>
     <row r="201" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A201" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B201" s="3" t="s">
         <v>177</v>
-      </c>
-      <c r="B201" s="3" t="s">
-        <v>187</v>
       </c>
       <c r="C201" s="3" t="s">
         <v>188</v>
@@ -7846,10 +7846,10 @@
       </c>
     </row>
     <row r="202" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A202" s="3" t="s">
+      <c r="A202" s="4"/>
+      <c r="B202" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B202" s="4"/>
       <c r="C202" s="4"/>
       <c r="D202" s="2" t="s">
         <v>180</v>
@@ -7877,10 +7877,10 @@
       </c>
     </row>
     <row r="203" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A203" s="3" t="s">
+      <c r="A203" s="4"/>
+      <c r="B203" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B203" s="4"/>
       <c r="C203" s="4"/>
       <c r="D203" s="2" t="s">
         <v>181</v>
@@ -7909,10 +7909,10 @@
     </row>
     <row r="204" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A204" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="B204" s="3" t="s">
         <v>177</v>
-      </c>
-      <c r="B204" s="3" t="s">
-        <v>189</v>
       </c>
       <c r="C204" s="3" t="s">
         <v>190</v>
@@ -7943,10 +7943,10 @@
       </c>
     </row>
     <row r="205" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A205" s="3" t="s">
+      <c r="A205" s="4"/>
+      <c r="B205" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B205" s="4"/>
       <c r="C205" s="4"/>
       <c r="D205" s="2" t="s">
         <v>180</v>
@@ -7975,10 +7975,10 @@
     </row>
     <row r="206" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A206" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B206" s="3" t="s">
         <v>177</v>
-      </c>
-      <c r="B206" s="3" t="s">
-        <v>191</v>
       </c>
       <c r="C206" s="3" t="s">
         <v>192</v>
@@ -8009,10 +8009,10 @@
       </c>
     </row>
     <row r="207" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A207" s="3" t="s">
+      <c r="A207" s="4"/>
+      <c r="B207" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B207" s="4"/>
       <c r="C207" s="4"/>
       <c r="D207" s="2" t="s">
         <v>180</v>
@@ -8041,10 +8041,10 @@
     </row>
     <row r="208" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A208" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B208" s="3" t="s">
         <v>177</v>
-      </c>
-      <c r="B208" s="3" t="s">
-        <v>193</v>
       </c>
       <c r="C208" s="3" t="s">
         <v>194</v>
@@ -8075,10 +8075,10 @@
       </c>
     </row>
     <row r="209" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A209" s="3" t="s">
+      <c r="A209" s="4"/>
+      <c r="B209" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B209" s="4"/>
       <c r="C209" s="4"/>
       <c r="D209" s="2" t="s">
         <v>180</v>
@@ -8106,10 +8106,10 @@
       </c>
     </row>
     <row r="210" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A210" s="3" t="s">
+      <c r="A210" s="4"/>
+      <c r="B210" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B210" s="4"/>
       <c r="C210" s="4"/>
       <c r="D210" s="2" t="s">
         <v>181</v>
@@ -8138,10 +8138,10 @@
     </row>
     <row r="211" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A211" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B211" s="3" t="s">
         <v>177</v>
-      </c>
-      <c r="B211" s="3" t="s">
-        <v>195</v>
       </c>
       <c r="C211" s="3" t="s">
         <v>196</v>
@@ -8172,10 +8172,10 @@
       </c>
     </row>
     <row r="212" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A212" s="3" t="s">
+      <c r="A212" s="4"/>
+      <c r="B212" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B212" s="4"/>
       <c r="C212" s="4"/>
       <c r="D212" s="2" t="s">
         <v>180</v>
@@ -8203,10 +8203,10 @@
       </c>
     </row>
     <row r="213" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A213" s="3" t="s">
+      <c r="A213" s="4"/>
+      <c r="B213" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B213" s="4"/>
       <c r="C213" s="4"/>
       <c r="D213" s="2" t="s">
         <v>181</v>
@@ -8235,10 +8235,10 @@
     </row>
     <row r="214" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A214" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B214" s="3" t="s">
         <v>177</v>
-      </c>
-      <c r="B214" s="3" t="s">
-        <v>197</v>
       </c>
       <c r="C214" s="3" t="s">
         <v>198</v>
@@ -8269,10 +8269,10 @@
       </c>
     </row>
     <row r="215" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A215" s="3" t="s">
+      <c r="A215" s="4"/>
+      <c r="B215" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B215" s="4"/>
       <c r="C215" s="4"/>
       <c r="D215" s="2" t="s">
         <v>180</v>
@@ -8300,10 +8300,10 @@
       </c>
     </row>
     <row r="216" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A216" s="3" t="s">
+      <c r="A216" s="4"/>
+      <c r="B216" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B216" s="4"/>
       <c r="C216" s="4"/>
       <c r="D216" s="2" t="s">
         <v>181</v>
@@ -8332,10 +8332,10 @@
     </row>
     <row r="217" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A217" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="B217" s="3" t="s">
         <v>177</v>
-      </c>
-      <c r="B217" s="3" t="s">
-        <v>199</v>
       </c>
       <c r="C217" s="3" t="s">
         <v>200</v>
@@ -8367,10 +8367,10 @@
     </row>
     <row r="218" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A218" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="B218" s="3" t="s">
         <v>177</v>
-      </c>
-      <c r="B218" s="3" t="s">
-        <v>201</v>
       </c>
       <c r="C218" s="3" t="s">
         <v>202</v>
@@ -8401,10 +8401,10 @@
       </c>
     </row>
     <row r="219" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A219" s="3" t="s">
+      <c r="A219" s="4"/>
+      <c r="B219" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B219" s="4"/>
       <c r="C219" s="4"/>
       <c r="D219" s="2" t="s">
         <v>180</v>
@@ -8432,10 +8432,10 @@
       </c>
     </row>
     <row r="220" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A220" s="3" t="s">
+      <c r="A220" s="4"/>
+      <c r="B220" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B220" s="4"/>
       <c r="C220" s="4"/>
       <c r="D220" s="2" t="s">
         <v>181</v>
@@ -8464,10 +8464,10 @@
     </row>
     <row r="221" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A221" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B221" s="3" t="s">
         <v>177</v>
-      </c>
-      <c r="B221" s="3" t="s">
-        <v>203</v>
       </c>
       <c r="C221" s="3" t="s">
         <v>204</v>
@@ -8498,10 +8498,10 @@
       </c>
     </row>
     <row r="222" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A222" s="3" t="s">
+      <c r="A222" s="4"/>
+      <c r="B222" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B222" s="4"/>
       <c r="C222" s="4"/>
       <c r="D222" s="2" t="s">
         <v>180</v>
@@ -8529,10 +8529,10 @@
       </c>
     </row>
     <row r="223" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A223" s="3" t="s">
+      <c r="A223" s="4"/>
+      <c r="B223" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B223" s="4"/>
       <c r="C223" s="4"/>
       <c r="D223" s="2" t="s">
         <v>181</v>
@@ -8561,10 +8561,10 @@
     </row>
     <row r="224" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A224" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B224" s="3" t="s">
         <v>177</v>
-      </c>
-      <c r="B224" s="3" t="s">
-        <v>205</v>
       </c>
       <c r="C224" s="3" t="s">
         <v>206</v>
@@ -8595,10 +8595,10 @@
       </c>
     </row>
     <row r="225" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A225" s="3" t="s">
+      <c r="A225" s="4"/>
+      <c r="B225" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B225" s="4"/>
       <c r="C225" s="4"/>
       <c r="D225" s="2" t="s">
         <v>180</v>
@@ -8626,10 +8626,10 @@
       </c>
     </row>
     <row r="226" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A226" s="3" t="s">
+      <c r="A226" s="4"/>
+      <c r="B226" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B226" s="4"/>
       <c r="C226" s="4"/>
       <c r="D226" s="2" t="s">
         <v>181</v>
@@ -8658,10 +8658,10 @@
     </row>
     <row r="227" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A227" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="B227" s="3" t="s">
         <v>177</v>
-      </c>
-      <c r="B227" s="3" t="s">
-        <v>207</v>
       </c>
       <c r="C227" s="3" t="s">
         <v>208</v>
@@ -8692,10 +8692,10 @@
       </c>
     </row>
     <row r="228" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A228" s="3" t="s">
+      <c r="A228" s="4"/>
+      <c r="B228" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B228" s="4"/>
       <c r="C228" s="4"/>
       <c r="D228" s="2" t="s">
         <v>180</v>
@@ -8723,10 +8723,10 @@
       </c>
     </row>
     <row r="229" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A229" s="3" t="s">
+      <c r="A229" s="4"/>
+      <c r="B229" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B229" s="4"/>
       <c r="C229" s="4"/>
       <c r="D229" s="2" t="s">
         <v>181</v>
@@ -8755,10 +8755,10 @@
     </row>
     <row r="230" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A230" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B230" s="3" t="s">
         <v>177</v>
-      </c>
-      <c r="B230" s="3" t="s">
-        <v>209</v>
       </c>
       <c r="C230" s="3" t="s">
         <v>210</v>
@@ -8789,10 +8789,10 @@
       </c>
     </row>
     <row r="231" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A231" s="3" t="s">
+      <c r="A231" s="4"/>
+      <c r="B231" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B231" s="4"/>
       <c r="C231" s="4"/>
       <c r="D231" s="2" t="s">
         <v>180</v>
@@ -8820,10 +8820,10 @@
       </c>
     </row>
     <row r="232" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A232" s="3" t="s">
+      <c r="A232" s="4"/>
+      <c r="B232" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B232" s="4"/>
       <c r="C232" s="4"/>
       <c r="D232" s="2" t="s">
         <v>181</v>
@@ -8852,10 +8852,10 @@
     </row>
     <row r="233" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A233" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B233" s="3" t="s">
         <v>177</v>
-      </c>
-      <c r="B233" s="3" t="s">
-        <v>211</v>
       </c>
       <c r="C233" s="3" t="s">
         <v>212</v>
@@ -8886,10 +8886,10 @@
       </c>
     </row>
     <row r="234" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A234" s="3" t="s">
+      <c r="A234" s="4"/>
+      <c r="B234" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B234" s="4"/>
       <c r="C234" s="4"/>
       <c r="D234" s="2" t="s">
         <v>180</v>
@@ -8917,10 +8917,10 @@
       </c>
     </row>
     <row r="235" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A235" s="3" t="s">
+      <c r="A235" s="4"/>
+      <c r="B235" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B235" s="4"/>
       <c r="C235" s="4"/>
       <c r="D235" s="2" t="s">
         <v>181</v>
@@ -8949,10 +8949,10 @@
     </row>
     <row r="236" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A236" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="B236" s="3" t="s">
         <v>177</v>
-      </c>
-      <c r="B236" s="3" t="s">
-        <v>213</v>
       </c>
       <c r="C236" s="3" t="s">
         <v>214</v>
@@ -8983,10 +8983,10 @@
       </c>
     </row>
     <row r="237" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A237" s="3" t="s">
+      <c r="A237" s="4"/>
+      <c r="B237" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B237" s="4"/>
       <c r="C237" s="4"/>
       <c r="D237" s="2" t="s">
         <v>180</v>
@@ -9014,10 +9014,10 @@
       </c>
     </row>
     <row r="238" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A238" s="3" t="s">
+      <c r="A238" s="4"/>
+      <c r="B238" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B238" s="4"/>
       <c r="C238" s="4"/>
       <c r="D238" s="2" t="s">
         <v>181</v>
@@ -9046,10 +9046,10 @@
     </row>
     <row r="239" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A239" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="B239" s="3" t="s">
         <v>177</v>
-      </c>
-      <c r="B239" s="3" t="s">
-        <v>215</v>
       </c>
       <c r="C239" s="3" t="s">
         <v>216</v>
@@ -9080,10 +9080,10 @@
       </c>
     </row>
     <row r="240" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A240" s="3" t="s">
+      <c r="A240" s="4"/>
+      <c r="B240" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B240" s="4"/>
       <c r="C240" s="4"/>
       <c r="D240" s="2" t="s">
         <v>180</v>
@@ -9111,10 +9111,10 @@
       </c>
     </row>
     <row r="241" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A241" s="3" t="s">
+      <c r="A241" s="4"/>
+      <c r="B241" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B241" s="4"/>
       <c r="C241" s="4"/>
       <c r="D241" s="2" t="s">
         <v>181</v>
@@ -9143,10 +9143,10 @@
     </row>
     <row r="242" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A242" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="B242" s="3" t="s">
         <v>177</v>
-      </c>
-      <c r="B242" s="3" t="s">
-        <v>217</v>
       </c>
       <c r="C242" s="3" t="s">
         <v>218</v>
@@ -9177,10 +9177,10 @@
       </c>
     </row>
     <row r="243" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A243" s="3" t="s">
+      <c r="A243" s="4"/>
+      <c r="B243" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B243" s="4"/>
       <c r="C243" s="4"/>
       <c r="D243" s="2" t="s">
         <v>180</v>
@@ -9208,10 +9208,10 @@
       </c>
     </row>
     <row r="244" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A244" s="3" t="s">
+      <c r="A244" s="4"/>
+      <c r="B244" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B244" s="4"/>
       <c r="C244" s="4"/>
       <c r="D244" s="2" t="s">
         <v>181</v>
@@ -9240,10 +9240,10 @@
     </row>
     <row r="245" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A245" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="B245" s="3" t="s">
         <v>177</v>
-      </c>
-      <c r="B245" s="3" t="s">
-        <v>219</v>
       </c>
       <c r="C245" s="3" t="s">
         <v>220</v>
@@ -9274,10 +9274,10 @@
       </c>
     </row>
     <row r="246" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A246" s="3" t="s">
+      <c r="A246" s="4"/>
+      <c r="B246" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B246" s="4"/>
       <c r="C246" s="4"/>
       <c r="D246" s="2" t="s">
         <v>180</v>
@@ -9305,10 +9305,10 @@
       </c>
     </row>
     <row r="247" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A247" s="3" t="s">
+      <c r="A247" s="4"/>
+      <c r="B247" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B247" s="4"/>
       <c r="C247" s="4"/>
       <c r="D247" s="2" t="s">
         <v>181</v>
@@ -9337,10 +9337,10 @@
     </row>
     <row r="248" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A248" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="B248" s="3" t="s">
         <v>177</v>
-      </c>
-      <c r="B248" s="3" t="s">
-        <v>221</v>
       </c>
       <c r="C248" s="3" t="s">
         <v>222</v>
@@ -9371,10 +9371,10 @@
       </c>
     </row>
     <row r="249" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A249" s="3" t="s">
+      <c r="A249" s="4"/>
+      <c r="B249" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B249" s="4"/>
       <c r="C249" s="4"/>
       <c r="D249" s="2" t="s">
         <v>180</v>
@@ -9402,10 +9402,10 @@
       </c>
     </row>
     <row r="250" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A250" s="3" t="s">
+      <c r="A250" s="4"/>
+      <c r="B250" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B250" s="4"/>
       <c r="C250" s="4"/>
       <c r="D250" s="2" t="s">
         <v>181</v>
@@ -9433,11 +9433,11 @@
       </c>
     </row>
     <row r="251" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A251" s="3" t="s">
+      <c r="A251" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="B251" s="3" t="s">
         <v>177</v>
-      </c>
-      <c r="B251" s="5" t="s">
-        <v>223</v>
       </c>
       <c r="C251" s="5" t="s">
         <v>224</v>
@@ -9468,10 +9468,10 @@
       </c>
     </row>
     <row r="252" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A252" s="3" t="s">
+      <c r="A252" s="4"/>
+      <c r="B252" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B252" s="4"/>
       <c r="C252" s="4"/>
       <c r="D252" s="2" t="s">
         <v>180</v>
@@ -9499,10 +9499,10 @@
       </c>
     </row>
     <row r="253" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A253" s="3" t="s">
+      <c r="A253" s="4"/>
+      <c r="B253" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B253" s="4"/>
       <c r="C253" s="4"/>
       <c r="D253" s="2" t="s">
         <v>181</v>
@@ -9531,10 +9531,10 @@
     </row>
     <row r="254" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A254" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="B254" s="3" t="s">
         <v>177</v>
-      </c>
-      <c r="B254" s="3" t="s">
-        <v>225</v>
       </c>
       <c r="C254" s="3" t="s">
         <v>226</v>
@@ -9565,10 +9565,10 @@
       </c>
     </row>
     <row r="255" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A255" s="3" t="s">
+      <c r="A255" s="4"/>
+      <c r="B255" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B255" s="4"/>
       <c r="C255" s="4"/>
       <c r="D255" s="2" t="s">
         <v>180</v>
@@ -9596,10 +9596,10 @@
       </c>
     </row>
     <row r="256" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A256" s="3" t="s">
+      <c r="A256" s="4"/>
+      <c r="B256" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B256" s="4"/>
       <c r="C256" s="4"/>
       <c r="D256" s="2" t="s">
         <v>181</v>
@@ -9628,10 +9628,10 @@
     </row>
     <row r="257" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A257" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="B257" s="3" t="s">
         <v>177</v>
-      </c>
-      <c r="B257" s="3" t="s">
-        <v>227</v>
       </c>
       <c r="C257" s="3" t="s">
         <v>228</v>
@@ -9662,10 +9662,10 @@
       </c>
     </row>
     <row r="258" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A258" s="3" t="s">
+      <c r="A258" s="4"/>
+      <c r="B258" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B258" s="4"/>
       <c r="C258" s="4"/>
       <c r="D258" s="2" t="s">
         <v>180</v>
@@ -9693,10 +9693,10 @@
       </c>
     </row>
     <row r="259" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A259" s="3" t="s">
+      <c r="A259" s="4"/>
+      <c r="B259" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B259" s="4"/>
       <c r="C259" s="4"/>
       <c r="D259" s="2" t="s">
         <v>181</v>
@@ -9725,10 +9725,10 @@
     </row>
     <row r="260" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A260" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="B260" s="3" t="s">
         <v>177</v>
-      </c>
-      <c r="B260" s="3" t="s">
-        <v>229</v>
       </c>
       <c r="C260" s="3" t="s">
         <v>230</v>
@@ -9759,10 +9759,10 @@
       </c>
     </row>
     <row r="261" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A261" s="3" t="s">
+      <c r="A261" s="4"/>
+      <c r="B261" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B261" s="4"/>
       <c r="C261" s="4"/>
       <c r="D261" s="2" t="s">
         <v>180</v>
@@ -9790,10 +9790,10 @@
       </c>
     </row>
     <row r="262" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A262" s="3" t="s">
+      <c r="A262" s="4"/>
+      <c r="B262" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B262" s="4"/>
       <c r="C262" s="4"/>
       <c r="D262" s="2" t="s">
         <v>181</v>
@@ -9822,10 +9822,10 @@
     </row>
     <row r="263" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A263" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="B263" s="3" t="s">
         <v>177</v>
-      </c>
-      <c r="B263" s="3" t="s">
-        <v>231</v>
       </c>
       <c r="C263" s="3" t="s">
         <v>232</v>
@@ -9856,10 +9856,10 @@
       </c>
     </row>
     <row r="264" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A264" s="3" t="s">
+      <c r="A264" s="4"/>
+      <c r="B264" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B264" s="4"/>
       <c r="C264" s="4"/>
       <c r="D264" s="2" t="s">
         <v>180</v>
@@ -9887,10 +9887,10 @@
       </c>
     </row>
     <row r="265" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A265" s="3" t="s">
+      <c r="A265" s="4"/>
+      <c r="B265" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B265" s="4"/>
       <c r="C265" s="4"/>
       <c r="D265" s="2" t="s">
         <v>181</v>
@@ -9919,10 +9919,10 @@
     </row>
     <row r="266" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A266" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="B266" s="3" t="s">
         <v>177</v>
-      </c>
-      <c r="B266" s="3" t="s">
-        <v>233</v>
       </c>
       <c r="C266" s="3" t="s">
         <v>234</v>
@@ -9953,10 +9953,10 @@
       </c>
     </row>
     <row r="267" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A267" s="3" t="s">
+      <c r="A267" s="4"/>
+      <c r="B267" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B267" s="4"/>
       <c r="C267" s="4"/>
       <c r="D267" s="2" t="s">
         <v>180</v>
@@ -9984,10 +9984,10 @@
       </c>
     </row>
     <row r="268" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A268" s="3" t="s">
+      <c r="A268" s="4"/>
+      <c r="B268" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B268" s="4"/>
       <c r="C268" s="4"/>
       <c r="D268" s="2" t="s">
         <v>181</v>
@@ -10016,10 +10016,10 @@
     </row>
     <row r="269" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A269" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="B269" s="3" t="s">
         <v>177</v>
-      </c>
-      <c r="B269" s="3" t="s">
-        <v>235</v>
       </c>
       <c r="C269" s="3" t="s">
         <v>236</v>
@@ -10050,10 +10050,10 @@
       </c>
     </row>
     <row r="270" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A270" s="3" t="s">
+      <c r="A270" s="4"/>
+      <c r="B270" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B270" s="4"/>
       <c r="C270" s="4"/>
       <c r="D270" s="2" t="s">
         <v>180</v>
@@ -10081,10 +10081,10 @@
       </c>
     </row>
     <row r="271" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A271" s="3" t="s">
+      <c r="A271" s="4"/>
+      <c r="B271" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B271" s="4"/>
       <c r="C271" s="4"/>
       <c r="D271" s="2" t="s">
         <v>181</v>
@@ -10113,10 +10113,10 @@
     </row>
     <row r="272" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A272" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="B272" s="3" t="s">
         <v>177</v>
-      </c>
-      <c r="B272" s="3" t="s">
-        <v>237</v>
       </c>
       <c r="C272" s="3" t="s">
         <v>238</v>
@@ -10147,10 +10147,10 @@
       </c>
     </row>
     <row r="273" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A273" s="3" t="s">
+      <c r="A273" s="4"/>
+      <c r="B273" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B273" s="4"/>
       <c r="C273" s="4"/>
       <c r="D273" s="2" t="s">
         <v>180</v>
@@ -10178,10 +10178,10 @@
       </c>
     </row>
     <row r="274" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A274" s="3" t="s">
+      <c r="A274" s="4"/>
+      <c r="B274" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B274" s="4"/>
       <c r="C274" s="4"/>
       <c r="D274" s="2" t="s">
         <v>181</v>
@@ -10209,10 +10209,10 @@
       </c>
     </row>
     <row r="275" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A275" s="6" t="s">
+      <c r="A275" s="7"/>
+      <c r="B275" s="6" t="s">
         <v>239</v>
       </c>
-      <c r="B275" s="7"/>
       <c r="C275" s="7"/>
       <c r="D275" s="7"/>
       <c r="E275" s="14"/>
@@ -10225,11 +10225,11 @@
       </c>
     </row>
     <row r="276" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A276" s="8" t="s">
+      <c r="A276" t="s">
+        <v>241</v>
+      </c>
+      <c r="B276" s="8" t="s">
         <v>240</v>
-      </c>
-      <c r="B276" t="s">
-        <v>241</v>
       </c>
       <c r="D276" s="9" t="s">
         <v>14</v>
@@ -10251,11 +10251,11 @@
       </c>
     </row>
     <row r="277" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A277" s="8" t="s">
+      <c r="A277" t="s">
+        <v>241</v>
+      </c>
+      <c r="B277" s="8" t="s">
         <v>240</v>
-      </c>
-      <c r="B277" t="s">
-        <v>241</v>
       </c>
       <c r="D277" s="9" t="s">
         <v>11</v>
@@ -10277,11 +10277,11 @@
       </c>
     </row>
     <row r="278" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A278" s="8" t="s">
+      <c r="A278" t="s">
+        <v>241</v>
+      </c>
+      <c r="B278" s="8" t="s">
         <v>240</v>
-      </c>
-      <c r="B278" t="s">
-        <v>241</v>
       </c>
       <c r="D278" s="9" t="s">
         <v>242</v>

</xml_diff>